<commit_message>
explanations and time vs g graph
</commit_message>
<xml_diff>
--- a/natural_frequency.xlsx
+++ b/natural_frequency.xlsx
@@ -673,16 +673,16 @@
         <v>-2.844083</v>
       </c>
       <c r="E10">
-        <v>-1885269</v>
+        <v>-1.885269</v>
       </c>
       <c r="F10">
         <v>0.4</v>
       </c>
       <c r="G10">
-        <v>-13.40434037849039</v>
+        <v>0.4111701794738866</v>
       </c>
       <c r="H10">
-        <v>-2.133367030123032</v>
+        <v>0.06543976651525081</v>
       </c>
       <c r="I10">
         <v>2.5</v>

</xml_diff>